<commit_message>
Update machine 2022-12-07 14:23
</commit_message>
<xml_diff>
--- a/files/templates/Machine_Report.xlsx
+++ b/files/templates/Machine_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\vidp\printerp\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\idp\erp\printerp\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7800153A-08B7-4621-B35F-8FBF34FF934C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87789EEF-8ABE-466B-857C-0500DC74879F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Item Code</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>TS/PIC Note</t>
+  </si>
+  <si>
+    <t>TS Note</t>
   </si>
 </sst>
 </file>
@@ -630,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL255"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2150,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E88686C-9756-408B-A0C1-92A9EBF8E9F3}">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2243,18 +2246,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6742AC-460E-4B55-BCD5-D23E5EC71FBF}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="15.7109375" customWidth="1"/>
+    <col min="1" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2278,6 +2279,9 @@
       </c>
       <c r="H1" s="12" t="s">
         <v>15</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new support performance.
</commit_message>
<xml_diff>
--- a/files/templates/Machine_Report.xlsx
+++ b/files/templates/Machine_Report.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\idp\erp\printerp\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87789EEF-8ABE-466B-857C-0500DC74879F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93F438-2DF1-4EB3-A96A-785AF427AEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$W$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Item Code</t>
   </si>
@@ -151,6 +152,12 @@
   </si>
   <si>
     <t>TS Note</t>
+  </si>
+  <si>
+    <t>Support Name</t>
+  </si>
+  <si>
+    <t>Over Time</t>
   </si>
 </sst>
 </file>
@@ -260,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,6 +301,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2150,6 +2160,840 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D2B0D2-A4B0-46CF-B280-36FF3F892F88}">
+  <dimension ref="A1:D255"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="9">
+        <f t="shared" ref="C1" si="0">SUBTOTAL(9, C4:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D1" s="10">
+        <f>SUMIF(D4:D20, "&lt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="str">
+        <f>COUNTIF(C4:C20, "=0") &amp; ":" &amp; COUNTIF(C4:C20, "&gt;0")</f>
+        <v>0:0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="11"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="11"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="11"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="11"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="11"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="11"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="11"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="11"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="11"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="11"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="11"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="11"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="11"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="11"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="11"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="11"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="11"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="8"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="8"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="8"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="8"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="8"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="8"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="8"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="8"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="8"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="8"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="8"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="8"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="8"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="8"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="8"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="8"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="8"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="8"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="8"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="8"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="8"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="8"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="8"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="8"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="8"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="8"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="8"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="8"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="8"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="8"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="8"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="8"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="8"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="8"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="8"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="8"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="8"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="8"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="8"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="8"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="8"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="8"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="8"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="8"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="8"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="8"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="8"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="8"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="8"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="8"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="8"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="8"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="8"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="8"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="8"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="8"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" s="8"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="8"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="8"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" s="8"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" s="8"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="8"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="8"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="8"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="8"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="8"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" s="8"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="8"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="8"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="8"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" s="8"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="8"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="8"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="8"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="8"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="8"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="8"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="8"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="8"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="8"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" s="8"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" s="8"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" s="8"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" s="8"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" s="8"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167" s="8"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168" s="8"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169" s="8"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170" s="8"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171" s="8"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" s="8"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D173" s="8"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D174" s="8"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D175" s="8"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D176" s="8"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D177" s="8"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D178" s="8"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D179" s="8"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D180" s="8"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D181" s="8"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D182" s="8"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D183" s="8"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D184" s="8"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D185" s="8"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D186" s="8"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D187" s="8"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D188" s="8"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D189" s="8"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D190" s="8"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D191" s="8"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D192" s="8"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D193" s="8"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D194" s="8"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195" s="8"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D196" s="8"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D197" s="8"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D198" s="8"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D199" s="8"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="8"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D201" s="8"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D202" s="8"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D203" s="8"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D204" s="8"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D205" s="8"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D206" s="8"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D207" s="8"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D208" s="8"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D209" s="8"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D210" s="8"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D211" s="8"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D212" s="8"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D213" s="8"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D214" s="8"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D215" s="8"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D216" s="8"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D217" s="8"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D218" s="8"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D219" s="8"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D220" s="8"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D221" s="8"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D222" s="8"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D223" s="8"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D224" s="8"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D225" s="8"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D226" s="8"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D227" s="8"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D228" s="8"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D229" s="8"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D230" s="8"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D231" s="8"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D232" s="8"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D233" s="8"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D234" s="8"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D235" s="8"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D236" s="8"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D237" s="8"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D238" s="8"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D239" s="8"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D240" s="8"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D241" s="8"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D242" s="8"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D243" s="8"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D244" s="8"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D245" s="8"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D246" s="8"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D247" s="8"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D248" s="8"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D249" s="8"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D250" s="8"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D251" s="8"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D252" s="8"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D253" s="8"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D254" s="8"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D255" s="8"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E88686C-9756-408B-A0C1-92A9EBF8E9F3}">
   <dimension ref="A1:W1"/>
   <sheetViews>
@@ -2244,7 +3088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6742AC-460E-4B55-BCD5-D23E5EC71FBF}">
   <dimension ref="A1:I1"/>
   <sheetViews>

</xml_diff>